<commit_message>
fix ml data loader
</commit_message>
<xml_diff>
--- a/files/test_ml_3.xlsx
+++ b/files/test_ml_3.xlsx
@@ -36,26 +36,26 @@
     <t xml:space="preserve">Вчера смотрел проститутку Тимошенко то ебется с адвокатом то со своим мужиком</t>
   </si>
   <si>
+    <t xml:space="preserve">мозги, конечно не видно,но когда их не хватает-ЗАМЕТНО :)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">а вот что такое ,,барокамера,,-я не знаю.....(((</t>
+  </si>
+  <si>
+    <t>Безысходность)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Когда же мой рабочий день кончится?...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Интересно у Параше остались самолёты и вертолеты или всех погрохали !Что-то они перестали летать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Майкоп 15.06.2013 время 23.20 град шел пол часа после сильнейшего  ливня, у всех в городе теперь крыши и капоты с вмятинами на машинах включая меня (((((((</t>
+  </si>
+  <si>
     <t xml:space="preserve">Маловато будет =(
 #ДеньРадио</t>
-  </si>
-  <si>
-    <t xml:space="preserve">мозги, конечно не видно,но когда их не хватает-ЗАМЕТНО :)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">а вот что такое ,,барокамера,,-я не знаю.....(((</t>
-  </si>
-  <si>
-    <t>Безысходность)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Когда же мой рабочий день кончится?...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Интересно у Параше остались самолёты и вертолеты или всех погрохали !Что-то они перестали летать</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Майкоп 15.06.2013 время 23.20 град шел пол часа после сильнейшего  ливня, у всех в городе теперь крыши и капоты с вмятинами на машинах включая меня (((((((</t>
   </si>
 </sst>
 </file>
@@ -650,42 +650,42 @@
       </c>
     </row>
     <row r="8" ht="71.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" ht="71.25">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" ht="14.25">
-      <c r="A15" s="2"/>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="2"/>

</xml_diff>

<commit_message>
fix bugs (order ds)
</commit_message>
<xml_diff>
--- a/files/test_ml_3.xlsx
+++ b/files/test_ml_3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>text</t>
   </si>
@@ -56,6 +56,9 @@
   <si>
     <t xml:space="preserve">Маловато будет =(
 #ДеньРадио</t>
+  </si>
+  <si>
+    <t>sm</t>
   </si>
 </sst>
 </file>
@@ -90,10 +93,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
@@ -709,7 +715,9 @@
       <c r="A22" s="2"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="2"/>

</xml_diff>